<commit_message>
Add a test case
The test case covers issues identified for the usage within
KernelHaven/IncrementalAnalysesInfrastructure
</commit_message>
<xml_diff>
--- a/testdata/test_input_linux/linux_ExpectedValues.xlsx
+++ b/testdata/test_input_linux/linux_ExpectedValues.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moritz/git/ComAn/testdata/test_input_linux/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{78BB6DE5-76D3-B743-9F2F-9C8E50325B73}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="14370"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28760" windowHeight="14380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="linux_ExpectedValues" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Commit</t>
   </si>
@@ -103,13 +109,16 @@
   </si>
   <si>
     <t>fbfbc48</t>
+  </si>
+  <si>
+    <t>incrementalProblems</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,15 +152,23 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -193,7 +210,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -225,9 +242,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -259,6 +294,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -434,28 +487,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -487,7 +540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -519,7 +572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -551,7 +604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -583,7 +636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -615,7 +668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -647,7 +700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -679,7 +732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -711,7 +764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -743,7 +796,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -775,7 +828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -807,7 +860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -839,7 +892,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
@@ -871,7 +924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -903,7 +956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -935,7 +988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -967,7 +1020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -999,7 +1052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -1031,7 +1084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -1063,7 +1116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1092,6 +1145,38 @@
         <v>0</v>
       </c>
       <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
         <v>0</v>
       </c>
     </row>
@@ -1102,24 +1187,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>